<commit_message>
New excel supports upto 5 ideas totally
</commit_message>
<xml_diff>
--- a/config/samples/teams_sample.xlsx
+++ b/config/samples/teams_sample.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,181 +509,225 @@
           <t>idea2_description</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>idea3_ps_title</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>idea3_ps_description</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>idea3_title</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>idea3_description</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>idea4_ps_title</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>idea4_ps_description</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>idea4_title</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>idea4_description</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>T001</t>
+          <t>Alpha Innovators</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alpha Innovators</t>
+          <t>PS-101</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>PS-101</t>
+          <t>Water Conservation</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Water Conservation</t>
+          <t>Smart Water Saver</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Smart Water Saver</t>
+          <t>Smart Drip System</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Smart Drip System</t>
+          <t>A low-cost IoT drip irrigation controller</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>A low-cost IoT drip irrigation controller</t>
+          <t>Air Quality</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Air Quality</t>
+          <t>Monitoring AQI in micro-climates</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Monitoring AQI in micro-climates</t>
+          <t>AirSense</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>AirSense</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
           <t>Portable AQI monitor prototype</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>T002</t>
+          <t>Beta Builders</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Beta Builders</t>
+          <t>PS-202</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>PS-202</t>
+          <t>Energy Efficiency</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Energy Efficiency</t>
+          <t>Home Energy Optimizer</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Home Energy Optimizer</t>
+          <t>HomeHub Energy Optimizer</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>HomeHub Energy Optimizer</t>
+          <t>Central controller for home energy management</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Central controller for home energy management</t>
+          <t>Waste Management</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Waste Management</t>
+          <t>Smart sorting bin</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Smart sorting bin</t>
+          <t>SmartSort</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>SmartSort</t>
+          <t>Automated waste sorting using sensors</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Automated waste sorting using sensors</t>
+          <t>Traffic Management</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Traffic Management</t>
+          <t>Adaptive signals</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>Adaptive signals</t>
+          <t>FlowSync</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>FlowSync</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
           <t>Traffic flow adaptive algorithm</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>T003</t>
+          <t>Gamma Tech</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Gamma Tech</t>
+          <t>PS-303</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PS-303</t>
+          <t>Healthcare Access</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Healthcare Access</t>
+          <t>TeleHealth Kiosk</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>TeleHealth Kiosk</t>
+          <t>TeleHealth Kiosk for rural clinics</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>TeleHealth Kiosk for rural clinics</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
           <t>Remote diagnostics and scheduling tool</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
@@ -692,6 +736,14 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>